<commit_message>
everything other than ai validate is ready some stuff need to be implemented
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,6 +442,11 @@
           <t>address</t>
         </is>
       </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>additional_feilds</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -457,7 +462,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>MD 59547, Port Laurenport, 36801 Kevin Harbors Apt. 656</t>
+          <t>36801 Kevin Harbors Apt. 656, Port Laurenport, MD 59547</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Unit ID : asdf123    Owner : Nice   </t>
         </is>
       </c>
     </row>
@@ -475,7 +485,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>MO 91646, Fergusonview, 50393 Jeremiah Ports</t>
+          <t>50393 Jeremiah Ports, Fergusonview, MO 91646</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Unit ID : asdf124    Owner : Nice   </t>
         </is>
       </c>
     </row>
@@ -493,7 +508,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>IA 91232, Sheilaborough, 8638 Wilson Overpass</t>
+          <t>8638 Wilson Overpass, Sheilaborough, IA 91232</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Unit ID : asdf125    Owner : Nice   </t>
         </is>
       </c>
     </row>
@@ -511,7 +531,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>OH 95791, North Tracyfurt, 627 Jeffrey Valleys</t>
+          <t>627 Jeffrey Valleys, North Tracyfurt, OH 95791</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Unit ID : asdf126    Owner : Nice   </t>
         </is>
       </c>
     </row>
@@ -529,7 +554,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>KS 49562, North Samantha, 024 Velazquez Lakes</t>
+          <t>024 Velazquez Lakes, North Samantha, KS 49562</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Unit ID : asdf127    Owner : Nice   </t>
         </is>
       </c>
     </row>
@@ -547,7 +577,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>KY 96338, Reidmouth, 2107 Mathews Mews Apt. 025</t>
+          <t>2107 Mathews Mews Apt. 025, Reidmouth, KY 96338</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Unit ID : asdf128    Owner : Nice   </t>
         </is>
       </c>
     </row>
@@ -565,7 +600,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>VT 98687, Biancahaven, 3573 Brown Gardens</t>
+          <t>3573 Brown Gardens, Biancahaven, VT 98687</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Unit ID : asdf129    Owner : Nice   </t>
         </is>
       </c>
     </row>
@@ -583,7 +623,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>GA 39886, Lake Yolanda, 3640 Flores Garden</t>
+          <t>3640 Flores Garden, Lake Yolanda, GA 39886</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Unit ID : asdf130    Owner : Nice   </t>
         </is>
       </c>
     </row>
@@ -601,7 +646,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>ND 71304, Hobbschester, 180 Burke Circle</t>
+          <t>180 Burke Circle, Hobbschester, ND 71304</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Unit ID : asdf132    Owner : Nice   </t>
         </is>
       </c>
     </row>
@@ -619,7 +669,12 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>OR 92406, Emilychester, 81384 Richard View Apt. 816</t>
+          <t>81384 Richard View Apt. 816, Emilychester, OR 92406</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Unit ID : asdf133    Owner : Nice   </t>
         </is>
       </c>
     </row>
@@ -637,7 +692,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>MI 90177, Lisaside, 042 Jamie Hollow</t>
+          <t>042 Jamie Hollow, Lisaside, MI 90177</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Unit ID : asdf135    Owner : Not Nice    </t>
         </is>
       </c>
     </row>
@@ -655,7 +715,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>NH 51356, North Lauraton, 36100 Horne Curve Apt. 345</t>
+          <t>36100 Horne Curve Apt. 345, North Lauraton, NH 51356</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Unit ID : asdf136    Owner : Not Nice    </t>
         </is>
       </c>
     </row>
@@ -673,7 +738,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>NH 99845, East Juanfurt, 20695 Vaughan Mountain</t>
+          <t>20695 Vaughan Mountain, East Juanfurt, NH 99845</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Unit ID : asdf137    Owner : Not Nice    </t>
         </is>
       </c>
     </row>
@@ -691,7 +761,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>IA 47964, Taylorshire, 6416 Hughes Forks Suite 776</t>
+          <t>6416 Hughes Forks Suite 776, Taylorshire, IA 47964</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Unit ID : asdf138    Owner : Not Nice    </t>
         </is>
       </c>
     </row>
@@ -709,7 +784,12 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>ID 31790, Deleonfurt, 11176 Sierra Greens Suite 643</t>
+          <t>11176 Sierra Greens Suite 643, Deleonfurt, ID 31790</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Unit ID : asdf139    Owner : Not Nice    </t>
         </is>
       </c>
     </row>
@@ -727,7 +807,12 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>PA 29774, Lake Donaldbury, 988 Vasquez Burgs</t>
+          <t>988 Vasquez Burgs, Lake Donaldbury, PA 29774</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Unit ID : asdf140    Owner : Not Nice    </t>
         </is>
       </c>
     </row>
@@ -745,7 +830,12 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>FL 51489, South Stephaniechester, 91896 Fleming Track</t>
+          <t>91896 Fleming Track, South Stephaniechester, FL 51489</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Unit ID : asdf141    Owner : Not Nice    </t>
         </is>
       </c>
     </row>
@@ -763,7 +853,12 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>MN 54161, Greenbury, 02638 Morrison Meadow</t>
+          <t>02638 Morrison Meadow, Greenbury, MN 54161</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Unit ID : asdf142    Owner : Not Nice    </t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
remake json feature now works(partially)
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,7 +466,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>E5V 8C4, 9998 Birch Blvd., Toronto, NL</t>
+          <t>L5M6N4, 9998 Birch Blvd., Toronto, NL</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -493,7 +493,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Q1E 8A5, 563 Queen St., St. John's, BC</t>
+          <t>M6H 9J0, 563 Queen St., St. John's, BC</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -520,7 +520,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>M4D 3M6, 3435 Cedar Ln., St. John's, AB</t>
+          <t>P0O9K8, 3435 Cedar Ln., St. John's, AB</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -547,370 +547,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>P5K 9D1, 1654 Queen St., Halifax, NB</t>
+          <t>P1K3L4, 1654 Queen St., Halifax, NB</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
           <t xml:space="preserve">Unit ID : unit-8443    Unit Type : Townhouse    Owner : Premium   </t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>jane.davis@example.com</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>+19123981617</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Jane Davis</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>E1R 7D4, 4947 Maple St., Regina, SK</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Unit ID : unit-4493    Unit Type : Apartment    Owner : Average   </t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>laura.williams@example.com</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>+18548441616</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Laura Williams</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>H6E 5K9, 119 Birch Blvd., Calgary, SK</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Unit ID : unit-3593    Unit Type : Detached    Owner : Average   </t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>sarah.jones@example.com</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>+19042519979</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Sarah Jones</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>O5V 8V7, 4899 Queen St., Vancouver, BC</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Unit ID : unit-6246    Unit Type : Condo    Owner : Average   </t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>laura.garcia@example.com</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>+17044542087</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Laura Garcia</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>R3V 2Y2, 134 Pine Ave., Winnipeg, MB</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Unit ID : unit-6634    Unit Type : Apartment    Owner : Average   </t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>emily.wilson@example.com</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Emily Wilson</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>O1Y 7P8, 7752 King Rd., Winnipeg, SK</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Unit ID : unit-2312    Unit Type : Semi-Detached    Owner : Premium   </t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>sarah.garcia@example.com</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Sarah Garcia</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>B7V 4K4, 3130 Elm Dr., Fredericton, SK</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Unit ID : unit-9120    Unit Type : Detached    Owner : Nice   </t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>alice.davis@example.com</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr"/>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Alice Davis</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>F4N 4S5, 4278 Elm Dr., Charlottetown, BC</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Unit ID : unit-6178    Unit Type : Apartment    Owner : Average   </t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>michael.wilson@example.com</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>+17043528923</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Michael Wilson</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>V2A 9U4, 579 King Rd., Regina, NL</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Unit ID : unit-3336    Unit Type : Semi-Detached    Owner : Great   </t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>robert.brown@example.com</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>+13418953748</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Robert Brown</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>J6D 8H4, 3200 Cedar Ln., Calgary, ON</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Unit ID : unit-2528    Unit Type : Semi-Detached    Owner : Average   </t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>laura.jones@example.com</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Laura Jones</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>L6K 9D8, 4483 Oak St., Fredericton, BC</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Unit ID : unit-7225    Unit Type : Apartment    Owner : Great   </t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>jane.wilson@example.com</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Jane Wilson</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>V6V 7J3, 9801 Elm Dr., Fredericton, NL</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Unit ID : unit-8228    Unit Type : Semi-Detached    Owner : Average   </t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>alice.miller@example.com</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>+19518053326</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Alice Miller</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>I9Q 6C3, 6029 Main St., Vancouver, ON</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Unit ID : unit-4586    Unit Type : Apartment    Owner : Average   </t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>michael.miller@example.com</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>+19703947116</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Michael Miller</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>F5C 8P8, 4258 Oak St., Toronto, PE</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Unit ID : unit-7298    Unit Type : Apartment    Owner : Premium   </t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>laura.williams@example.com</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>+15347418866</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Laura Williams</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>R9S 4C1, 1685 Queen St., Charlottetown, NL</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Unit ID : unit-8857    Unit Type : Semi-Detached    Owner : Average   </t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Importing Remake.json files back to the output.xlsx
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -26,12 +26,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D9D9D9"/>
+        <bgColor rgb="00D9D9D9"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -46,8 +52,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -556,6 +563,283 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" s="1" t="n"/>
+      <c r="B6" s="1" t="n"/>
+      <c r="C6" s="1" t="n"/>
+      <c r="D6" s="1" t="n"/>
+      <c r="E6" s="1" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>daniel.williams@example.com</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>416 715 6897</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Daniel Williams</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>766 Birch Blvd., L8K7J6, Charletown, PE, US</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Unit ID : unit-4970    Unit Type : Apartment    Owner : Great   </t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>jane.davis@example.com</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>416 715 6897</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Jane Davis</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>4947 Maple St., L5K7J6, Regina, SK, US</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Unit ID : unit-4493    Unit Type : Apartment    Owner : Average   </t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>jane.davis@example.com</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>416 715 6897</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Jane Davis</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>4947 Maple St., L5K7J6, Regina, SK, US</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Unit ID : unit-4493    Unit Type : Apartment    Owner : Average   </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>jane.davis@example.com</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>416 715 6897</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Jane Davis</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>4947 Maple St., L5K7J6, Regina, SK, US</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Unit ID : unit-4493    Unit Type : Apartment    Owner : Average   </t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>jane.davis@example.com</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>416 715 6897</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Jane Davis</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>4947 Maple St., L5K7J6, Regina, SK, US</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Unit ID : unit-4493    Unit Type : Apartment    Owner : Average   </t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>jane.davis@example.com</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>416 715 6897</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Jane Davis</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>4947 Maple St., L5K7J6, Regina, SK, US</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Unit ID : unit-4493    Unit Type : Apartment    Owner : Average   </t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>jane.davis@example.com</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>416 715 6897</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Jane Davis</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>4947 Maple St., L5K7J6, Regina, SK, US</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Unit ID : unit-4493    Unit Type : Apartment    Owner : Average   </t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>jane.davis@example.com</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>416 715 6897</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Jane Davis</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>4947 Maple St., L5K7J6, Regina, SK, US</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Unit ID : unit-4493    Unit Type : Apartment    Owner : Average   </t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>jane.davis@example.com</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>416 715 6897</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Jane Davis</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>4947 Maple St., L5K7J6, Regina, SK, US</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Unit ID : unit-4493    Unit Type : Apartment    Owner : Average   </t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>jane.davis@example.com</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>416 715 6897</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Jane Davis</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>4947 Maple St., L5K7J6, Regina, SK, US</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Unit ID : unit-4493    Unit Type : Apartment    Owner : Average   </t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Merged all parts together, need to work on ai format and geopy for single coulmn addresses
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -26,12 +26,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D9D9D9"/>
+        <bgColor rgb="00D9D9D9"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -46,8 +52,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,7 +463,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>+18733083608</t>
+          <t>8733083608</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -483,7 +490,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>+19753501446</t>
+          <t>9753501446</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -510,7 +517,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>+13544172164</t>
+          <t>3544172164</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -537,7 +544,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>+17713556101</t>
+          <t>7713556101</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -555,6 +562,132 @@
           <t xml:space="preserve">Unit ID : unit-8443    Unit Type : Townhouse    Owner : Premium   </t>
         </is>
       </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>jane.taylor@example.com</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>8733083608</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Jane Taylor</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>daniel.williams@example.com</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>9753501446</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Daniel Williams</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>jane.williams@example.com</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>3544172164</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Jane Williams</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>daniel.williams@example.com</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>6646753997</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Daniel Williams</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>alice.williams@example.com</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>7713556101</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Alice Williams</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>jane.davis@example.com</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>9123981617</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Jane Davis</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>jane.davis@example.com</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>9123981618</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Jane Davis</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n"/>
+      <c r="B13" s="1" t="n"/>
+      <c r="C13" s="1" t="n"/>
+      <c r="D13" s="1" t="n"/>
+      <c r="E13" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Backup Version for Friday
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -431,32 +431,32 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>email</t>
+          <t>Full Name</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>phone_number</t>
+          <t>Phone Number</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>full_name</t>
+          <t>Email</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>shipping_address</t>
+          <t>Billing Address</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>billing_address</t>
+          <t>Shipping Address</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>additional_fields</t>
+          <t>Additional Feilds</t>
         </is>
       </c>
     </row>
@@ -471,13 +471,13 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>invoices@tphinc.ca</t>
+          <t>Invoices</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Invoices</t>
+          <t>invoices@tphinc.ca</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -499,23 +499,23 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>david@stoneworks.ca</t>
+          <t>David</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>David</t>
+          <t>david@stoneworks.ca</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>5586 Pettapiece Crescent, Manotick, Ontario, Canada, K4M 1C5</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>Orleans Vacuums, 2742, St. Joseph Boulevard, Orléans Village - Châteauneuf, Orléans, Orléans East-Cumberland, Ottawa, Eastern Ontario, Ontario, K1C 1G5, Canada</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>5586 Pettapiece Crescent, Manotick, Ontario, Canada, K4M 1C5</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -527,27 +527,27 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>Karl</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Phone:613-875-5275</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>karl@lakadd.com</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Phone:613-875-5275</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Karl</t>
-        </is>
-      </c>
       <c r="D5" t="inlineStr">
         <is>
+          <t>1556 St-Joseph, Embrun, ON, Canada, K0A 1W0</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>Unable to extract address</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>1556 St-Joseph, Embrun, ON, Canada, K0A 1W0</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -559,13 +559,13 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>1150107 Ontario Inc.</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1150107 Ontario Inc.</t>
+          <t>MISSING</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -587,17 +587,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>Xavier</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Phone:819-243-3306</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>xavier@portesltr.com</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Phone:819-243-3306</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Xavier</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -619,27 +619,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>1729management</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Phone:613-224-4488</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
           <t>1729.management@hotmail.ca</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Phone:613-224-4488</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>1729management</t>
-        </is>
-      </c>
       <c r="D8" t="inlineStr">
         <is>
+          <t>6, Dalecroft Crescent, Centrepointe, College, Nepean, Ottawa, Eastern Ontario, Ontario, K2G 5K7, Canada</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>Unable to extract address</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>6, Dalecroft Crescent, Centrepointe, College, Nepean, Ottawa, Eastern Ontario, Ontario, K2G 5K7, Canada</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -651,7 +651,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>SWood@pattenhomes.com</t>
+          <t>Swood</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -661,17 +661,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Swood</t>
+          <t>swood@pattenhomes.com</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
+          <t>9094 Cavanagh Rd, Ashton, Ontario, Canada, K0A 1B0</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
           <t>707, Ploughman Place, Stittsville, Ottawa, Eastern Ontario, Ontario, K2S 1K5, Canada</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>9094 Cavanagh Rd, Ashton, Ontario, Canada, K0A 1B0</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -683,13 +683,13 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>pph@pphinc.ca</t>
+          <t>No Name</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr">
         <is>
-          <t>No Name</t>
+          <t>pph@pphinc.ca</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -711,23 +711,23 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>invoices@tphinc.ca</t>
+          <t>Invoices</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Invoices</t>
+          <t>invoices@tphinc.ca</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
+          <t>1528 Startop Rd, Ottawa, Ontario, Canada, K1B 3W6</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
           <t>Unable to extract address</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>1528 Startop Rd, Ottawa, Ontario, Canada, K1B 3W6</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -739,13 +739,13 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>accounting@appletreemedicalgroup.com</t>
+          <t>No Name</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr">
         <is>
-          <t>No Name</t>
+          <t>accounting@appletreemedicalgroup.com</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -767,12 +767,13 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>Laprile1947</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr">
+        <is>
           <t>l.aprile1947@gmail.com</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Laprile1947</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -794,27 +795,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>Kaichen5</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Phone:416-520-4898</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
           <t>kaichen5@gmail.com</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Phone:416-520-4898</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Kaichen5</t>
-        </is>
-      </c>
       <c r="D14" t="inlineStr">
         <is>
+          <t>20 Rolark Dr. Unit 1, Scarborough, Ontario, Canada, M1R 4G2</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
           <t>175, McArthur Avenue, Vanier, Rideau-Vanier, Ottawa, Eastern Ontario, Ontario, K1L 6P8, Canada</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>20 Rolark Dr. Unit 1, Scarborough, Ontario, Canada, M1R 4G2</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -826,17 +827,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>Scottlanecan</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Phone:613-295-3954</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
           <t>scottlanecan@hotmail.com</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Phone:613-295-3954</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Scottlanecan</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -858,17 +859,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>Govind</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Phone:613-596-9663 Mobile:613-482-2810</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
           <t>govind@kionas.ca</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Phone:613-596-9663 Mobile:613-482-2810</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Govind</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -890,17 +891,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>90kinggan</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Phone:343-364-9005</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
           <t>90kinggan@gmail.com</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Phone:343-364-9005</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>90kinggan</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -922,22 +923,23 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>No Name</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr">
+        <is>
           <t>dbourdon@carefor.ca</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>No Name</t>
-        </is>
-      </c>
       <c r="D18" t="inlineStr">
         <is>
+          <t>205 Amelia Street, Cornwall, Ontario, Canada, K6H 3P3</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
           <t>1026, Rue Laurier Street, Rockland, Clarence-Rockland, Prescott and Russell Counties, Eastern Ontario, Ontario, K4K 1K6, Canada</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>205 Amelia Street, Cornwall, Ontario, Canada, K6H 3P3</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -949,7 +951,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>2075227 Ontario Inc.</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -959,7 +961,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2075227 Ontario Inc.</t>
+          <t>MISSING</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -981,12 +983,13 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Demers.realspace@rogers.com</t>
-        </is>
-      </c>
+          <t>Demersrealspace</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Demersrealspace</t>
+          <t>demers.realspace@rogers.com</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1008,7 +1011,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>20 Vic Management Inc.</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1018,7 +1021,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>20 Vic Management Inc.</t>
+          <t>MISSING</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1040,12 +1043,13 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
+          <t>2135560 Ontario Limited</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2135560 Ontario Limited</t>
+          <t>MISSING</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1067,17 +1071,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>2164613 Ontario Inc.</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Phone:</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2164613 Ontario Inc.</t>
+          <t>MISSING</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1099,17 +1103,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
+          <t>2241497 Ontario Limited</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Phone:(613) 227-7997 Fax:(613) 256-8998</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
           <t>rodayotte@yahoo.ca</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Phone:(613) 227-7997 Fax:(613) 256-8998</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>2241497 Ontario Limited</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1131,7 +1135,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Rodayotte@yahoo.ca, sveta@elmdevelopments.com, d.osypowich@elmdevelopments.com</t>
+          <t>Rodayotte</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1141,17 +1145,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Rodayotte</t>
+          <t>rodayotte@yahoo.ca, sveta@elmdevelopments.com, d.osypowich@elmdevelopments.com</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
+          <t>c/o 2241497 Ontario Limited Concord Ontario L4K 1V5 c/o Jason D'Elia                      Attention: Accounts Payable, Concord, Ontario, Canada, L4K 1V5</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
           <t>Unable to extract address</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>c/o 2241497 Ontario Limited Concord Ontario L4K 1V5 c/o Jason D'Elia, Concord, Ontario, Canada, L4K 1V5</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1163,27 +1167,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
+          <t>Snovak</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Phone:613-831-0700</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
           <t>snovak@bergrealty.ca</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Phone:613-831-0700</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Snovak</t>
-        </is>
-      </c>
       <c r="D26" t="inlineStr">
         <is>
+          <t>106 Westover Crescent, Ottawa, ON, Canada, K2T 0K6</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
           <t>Missing</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>106 Westover Crescent, Ottawa, ON, Canada, K2T 0K6</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1205,17 +1209,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>MISSING</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
+          <t>Missing</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
           <t>242 Rideau Street, Ottawa, ON, Canada, K1N 5Y3</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>Missing</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1227,17 +1231,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>2553395 Ontario Inc.</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Phone:</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2553395 Ontario Inc.</t>
+          <t>MISSING</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1259,27 +1263,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
+          <t>No Name</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Phone:</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
           <t>invoices@hein.ca</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>No Name</t>
-        </is>
-      </c>
       <c r="D29" t="inlineStr">
         <is>
+          <t>275, Michael Cowpland Drive, Kanata, Kanata South, Ottawa, Eastern Ontario, Ontario, K2M 0E2, Canada</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
           <t>Missing</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>275, Michael Cowpland Drive, Kanata, Kanata South, Ottawa, Eastern Ontario, Ontario, K2M 0E2, Canada</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1301,7 +1305,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>MISSING</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1333,7 +1337,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>MISSING</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1365,7 +1369,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>MISSING</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1397,17 +1401,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>MISSING</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
+          <t>Missing</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
           <t>705 Mackay St, Pembroke, , Canada, K8A 1G8</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>None, None, , None, None</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -1419,7 +1423,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>2950-2960 Bank St. Retail Centre</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1429,7 +1433,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2950-2960 Bank St. Retail Centre</t>
+          <t>MISSING</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1451,17 +1455,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
+          <t>2c London</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
           <t>None</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2c London</t>
+          <t>MISSING</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1483,27 +1487,27 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
+          <t>Payables</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Phone:613-736-7807 ext 121</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
           <t>payables@sentinelmanagement.com</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>Phone:613-736-7807 ext 121</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>Payables</t>
-        </is>
-      </c>
       <c r="D36" t="inlineStr">
         <is>
+          <t>5832 Bank Street, Ottawa, , Canada, K4P 1B9</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
           <t>310 Centrum Blvd, Orleans, , Canada, K1E 3W8</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>5832 Bank Street, Ottawa, , Canada, K4P 1B9</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -1515,7 +1519,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>3181642 Canada Inc.</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1525,7 +1529,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>3181642 Canada Inc.</t>
+          <t>MISSING</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1547,17 +1551,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
+          <t>360 Advanced Security Corp.</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
           <t>serviceottawa@360asc.com</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>360 Advanced Security Corp.</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1579,17 +1583,17 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
+          <t>3673928 Canada Inc.</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
           <t>None</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>3673928 Canada Inc.</t>
+          <t>MISSING</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1611,27 +1615,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
+          <t>Schryver3f</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
           <t>schryver3f@hotmail.ca</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>Schryver3f</t>
-        </is>
-      </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>3541 Dalmac Rd, Osgoode, , None, None</t>
+          <t>3541, Dalmac Road, Dalmeny, Osgoode, Ottawa, Eastern Ontario, Ontario, Canada</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>3541 Dalmac Rd, Osgoode, , None, None</t>
+          <t>3541, Dalmac Road, Dalmeny, Osgoode, Ottawa, Eastern Ontario, Ontario, Canada</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -1643,17 +1647,17 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
+          <t>Me</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Phone:613-342-6042</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
           <t>me@me.com</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>Phone:613-342-6042</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>Me</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1675,27 +1679,27 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
+          <t>Info</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Phone:613-264-6135  - Earl Kerr</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
           <t>info@rgss-ventures.com</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>Phone:613-264-6135  - Earl Kerr</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>Info</t>
-        </is>
-      </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>40 Sunset Blvd., None, , None, None</t>
+          <t>The Factory, 40, Sunset Boulevard, Perth, Lanark County, Eastern Ontario, Ontario, K7H 2P8, Canada</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>40 Sunset Blvd., Perth, , None, None</t>
+          <t>Missing</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -1717,17 +1721,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>MISSING</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
+          <t>Missing</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
           <t>Perth, City of Perth, Western Australia, 6000, Australia</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>Missing</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -1739,17 +1743,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
+          <t>415 Legget Leaseholds Inc.</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
           <t>None</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>415 Legget Leaseholds Inc.</t>
+          <t>MISSING</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1771,17 +1775,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
+          <t>4site Retail Services Inc.</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
           <t>None</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>4site Retail Services Inc.</t>
+          <t>MISSING</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1803,17 +1807,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
+          <t>Ottawahandymanservicesca</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
           <t>ottawahandymanservices.ca@gmail.com</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>Ottawahandymanservicesca</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1835,17 +1839,17 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
+          <t>Stephspin</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Phone:613-229-4485 - Charlie</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
           <t>stephspin@gmail.com</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>Phone:613-229-4485 - Charlie</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>Stephspin</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1867,17 +1871,17 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
+          <t>No Name</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Phone:613-225-7663</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
           <t>cneville@aquatopiaconservatory.com</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>Phone:613-225-7663</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>No Name</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1899,17 +1903,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
+          <t>No Name</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Phone:613-299-1979</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
           <t>ccbelda@gmail.com</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>Phone:613-299-1979</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>No Name</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1931,17 +1935,17 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
+          <t>No Name</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Phone:613-445-2944</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
           <t>beth@frecon.ca</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>Phone:613-445-2944</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>No Name</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1963,27 +1967,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
+          <t>Khanes</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
           <t>k.hanes@frecon.ca</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>Khanes</t>
-        </is>
-      </c>
       <c r="D51" t="inlineStr">
         <is>
+          <t>1235 South Russell Rd., Russell, Ontario, None, K4R 1E1</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
           <t>Unable to extract address</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>1235 South Russell Rd., Russell, Ontario, None, K4R 1E1</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -1995,27 +1999,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
+          <t>Accounting</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
           <t>accounting@frecon.ca, beth@frecon.ca, m.jones@frecon.ca</t>
         </is>
       </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>Accounting</t>
-        </is>
-      </c>
       <c r="D52" t="inlineStr">
         <is>
+          <t>1235 South Russell Road, Box 278, Russell, Ontario, None, K4R 1E1</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
           <t>Unable to extract address</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>1235 South Russell Road, Box 278, Russell, Ontario, None, K4R 1E1</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -2027,23 +2031,23 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>accounting@frecon.ca, beth@frecon.ca, m.jones@frecon.ca</t>
+          <t>Accounting</t>
         </is>
       </c>
       <c r="B53" t="inlineStr"/>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Accounting</t>
+          <t>accounting@frecon.ca, beth@frecon.ca, m.jones@frecon.ca</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
+          <t>1235 South Russell Road, Box 278, Russell, Ontario, Canada, K4R 1E1</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
           <t>Clifford Bowey Public School, 1300, Kitchener Avenue, Ellwood, River, Ottawa, Eastern Ontario, Ontario, K1V 6W2, Canada</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>1235 South Russell Road, Box 278, Russell, Ontario, Canada, K4R 1E1</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -2055,23 +2059,23 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>accounting@frecon.ca, beth@frecon.ca, m.jones@frecon.ca</t>
+          <t>Accounting</t>
         </is>
       </c>
       <c r="B54" t="inlineStr"/>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Accounting</t>
+          <t>accounting@frecon.ca, beth@frecon.ca, m.jones@frecon.ca</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
+          <t>1235 South Russell Road, Box 278, Russell, Ontario, None, K4R 1E1</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
           <t>480 Cope Drive, Ottawa, Ontario, None, K2V 0B8</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>1235 South Russell Road, Box 278, Russell, Ontario, None, K4R 1E1</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -2083,27 +2087,27 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
+          <t>Accounting</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Phone:613-445-2944</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
           <t>accounting@frecon.ca, beth@frecon.ca, m.jones@frecon.ca</t>
         </is>
       </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>Phone:613-445-2944</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>Accounting</t>
-        </is>
-      </c>
       <c r="D55" t="inlineStr">
         <is>
+          <t>1235 South Russell Road, Box 278, Russell, Ontario, None, K4R 1E1</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
           <t>Gloucester High School, 2060, Ogilvie Road, Gloucester, Beacon Hill-Cyrville, Ottawa, Eastern Ontario, Ontario, K1J 7N8, Canada</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>1235 South Russell Road, Box 278, Russell, Ontario, None, K4R 1E1</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -2115,23 +2119,23 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>accounting@frecon.ca, beth@frecon.ca, m.jones@frecon.ca</t>
+          <t>Accounting</t>
         </is>
       </c>
       <c r="B56" t="inlineStr"/>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Accounting</t>
+          <t>accounting@frecon.ca, beth@frecon.ca, m.jones@frecon.ca</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
+          <t>1235 South Russell Road, Box 278, Russell, Ontario, Canada, K4R 1E1</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
           <t>Goulbourn Middle School, 2176, Huntley Road, Stanley Corners, Rideau-Jock, Ottawa, Eastern Ontario, Ontario, K2S 1B8, Canada</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>1235 South Russell Road, Box 278, Russell, Ontario, Canada, K4R 1E1</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -2143,23 +2147,23 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>accounting@frecon.ca, beth@frecon.ca, m.jones@frecon.ca</t>
+          <t>Accounting</t>
         </is>
       </c>
       <c r="B57" t="inlineStr"/>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Accounting</t>
+          <t>accounting@frecon.ca, beth@frecon.ca, m.jones@frecon.ca</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
+          <t>1235 South Russell Rd., Russell, Ontario, None, K4R 1E1</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
           <t>2025, Lanthier Drive, Avalon, Orléans, Orléans South-Navan, Ottawa, Eastern Ontario, Ontario, K4A 3V5, Canada</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>1235 South Russell Rd., Russell, Ontario, None, K4R 1E1</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -2171,23 +2175,23 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>accounting@frecon.ca, beth@frecon.ca, m.jones@frecon.ca</t>
+          <t>Accounting</t>
         </is>
       </c>
       <c r="B58" t="inlineStr"/>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Accounting</t>
+          <t>accounting@frecon.ca, beth@frecon.ca, m.jones@frecon.ca</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
+          <t>1235 South Russell Road, Box 278, Russell, Ontario, None, K4R 1E1</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
           <t>170, Greenbank Road, Craig Henry, Knoxdale-Merivale, Nepean, Ottawa, Eastern Ontario, Ontario, K2H 5V2, Canada</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>1235 South Russell Road, Box 278, Russell, Ontario, None, K4R 1E1</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -2199,23 +2203,23 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>k.hanes@frecon.ca</t>
+          <t>Khanes</t>
         </is>
       </c>
       <c r="B59" t="inlineStr"/>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Khanes</t>
+          <t>k.hanes@frecon.ca</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
+          <t>1235 South Russell Rd., Russell, Ontario, Canada, K4R 1E1</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
           <t>Metcalfe Public School, 2701, 8th Line Road, Metcalfe, Ottawa, Eastern Ontario, Ontario, K0A 2P0, Canada</t>
-        </is>
-      </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>1235 South Russell Rd., Russell, Ontario, Canada, K4R 1E1</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -2227,27 +2231,27 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
+          <t>Accounting</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Phone:613-445-2944</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
           <t>accounting@frecon.ca, beth@frecon.ca, m.jones@frecon.ca</t>
         </is>
       </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>Phone:613-445-2944</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>Accounting</t>
-        </is>
-      </c>
       <c r="D60" t="inlineStr">
         <is>
+          <t>1235 South Russell Road, Box 278, Russell, Ontario, None, K4R 1E1</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
           <t>Sir Wilfrid Laurier Secondary School, 1515, Tenth Line Road, Fallingbrook, Orléans, Orléans East-Cumberland, Ottawa, Eastern Ontario, Ontario, K1E 3E8, Canada</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>1235 South Russell Road, Box 278, Russell, Ontario, None, K4R 1E1</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -2259,17 +2263,17 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
+          <t>No Name</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Phone:613-714-1110</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
           <t>accounts@aquatria.ca</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>Phone:613-714-1110</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>No Name</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2291,27 +2295,27 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
+          <t>No Name</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Phone:613-733-7507</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
           <t>scott@mminterior.ca</t>
         </is>
       </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>Phone:613-733-7507</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>No Name</t>
-        </is>
-      </c>
       <c r="D62" t="inlineStr">
         <is>
+          <t>861, Boyd Avenue, McKellar Heights, Bay, Ottawa, Eastern Ontario, Ontario, K2A 2C5, Canada</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
           <t>255 Albert St, Ottawa, Ontario, Canada, K1P 6A9</t>
-        </is>
-      </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>861, Boyd Avenue, McKellar Heights, Bay, Ottawa, Eastern Ontario, Ontario, K2A 2C5, Canada</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -2323,17 +2327,17 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
+          <t>No Name</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Phone:613-804-9028</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
           <t>sabbi@premium-construction.ca</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>Phone:613-804-9028</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>No Name</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -2355,22 +2359,22 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Tania@premium-construction.ca, sabbi@premium-construction.ca, admin@premium-construction.ca</t>
+          <t>Tania</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Tania</t>
+          <t>tania@premium-construction.ca, sabbi@premium-construction.ca, admin@premium-construction.ca</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
+          <t>P.O. Box 45057, Kanata South, Kanata, Canada, K2M 2Y1</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
           <t>A&amp;W, Main Street West, Winchester, North Dundas, Stormont, Dundas and Glengarry Counties, Eastern Ontario, Ontario, K0C 2K0, Canada</t>
-        </is>
-      </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>P.O. Box 45057, Kanata South, Kanata, Canada, K2M 2Y1</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -2382,22 +2386,22 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Tania@premium-construction.ca, sabbi@premium-construction.ca, admin@premium-construction.ca</t>
+          <t>Tania</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Tania</t>
+          <t>tania@premium-construction.ca, sabbi@premium-construction.ca, admin@premium-construction.ca</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
+          <t>P.O. Box 45057, Kanata South, Kanata, Canada, K2M 2Y1</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
           <t>Unable to extract address</t>
-        </is>
-      </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>P.O. Box 45057, Kanata South, Kanata, Canada, K2M 2Y1</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -2409,17 +2413,17 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
+          <t>No Name</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Phone:613-822-6594</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
           <t>kyle@blackforestcontractor.ca</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>Phone:613-822-6594</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>No Name</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2441,17 +2445,17 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
+          <t>No Name</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Phone:613-831-2383</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
           <t>goulbourn@bellnet.ca</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>Phone:613-831-2383</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>No Name</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2473,27 +2477,27 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
+          <t>No Name</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Phone:613-831-2383</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
           <t>goulbourn@bellnet.ca</t>
         </is>
       </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>Phone:613-831-2383</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>No Name</t>
-        </is>
-      </c>
       <c r="D68" t="inlineStr">
         <is>
+          <t>Carleton Apartments, 1, Carleton Cathcart Street, Stittsville, Ottawa, Eastern Ontario, Ontario, K2S 1A2, Canada</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
           <t>126, Hamilton Street, Hamlet, Richmond County, North Carolina, 28345, United States</t>
-        </is>
-      </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>Carleton Apartments, 1, Carleton Cathcart Street, Stittsville, Ottawa, Eastern Ontario, Ontario, K2S 1A2, Canada</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -2505,17 +2509,17 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
+          <t>Billing6172199canadainc</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Phone:613-323-5914</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
           <t>billing.6172199canadainc@gmail.com</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>Phone:613-323-5914</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>Billing6172199canadainc</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2537,27 +2541,27 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
+          <t>Billing6172199canadainc</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Phone:613-723-5719</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
           <t>billing.6172199canadainc@gmail.com</t>
         </is>
       </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>Phone:613-723-5719</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>Billing6172199canadainc</t>
-        </is>
-      </c>
       <c r="D70" t="inlineStr">
         <is>
+          <t>1675 Merivale Rd, Ottawa, Ontario, Canada, K2G 3K2</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
           <t>Unable to extract address</t>
-        </is>
-      </c>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>1675 Merivale Rd, Ottawa, Ontario, Canada, K2G 3K2</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -2569,27 +2573,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
+          <t>Billing6172199canadainc</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Phone:613-323-5914</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
           <t>billing.6172199canadainc@gmail.com</t>
         </is>
       </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>Phone:613-323-5914</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>Billing6172199canadainc</t>
-        </is>
-      </c>
       <c r="D71" t="inlineStr">
         <is>
+          <t>1675 Merivale Rd., Ottawa, Ontario, None, K2G 3K2</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
           <t>Missing</t>
-        </is>
-      </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>1675 Merivale Rd., Ottawa, Ontario, None, K2G 3K2</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -2606,17 +2610,17 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>MISSING</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
+          <t>Missing</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
           <t>Unable to extract address</t>
-        </is>
-      </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>Missing</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">

</xml_diff>